<commit_message>
Designing procedural generation algorithm.
</commit_message>
<xml_diff>
--- a/Zone1Study.xlsx
+++ b/Zone1Study.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="90" windowWidth="22995" windowHeight="14640" activeTab="2"/>
+    <workbookView xWindow="120" yWindow="90" windowWidth="22995" windowHeight="14640"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="251" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="366" uniqueCount="46">
   <si>
     <t>T</t>
   </si>
@@ -61,6 +61,99 @@
   </si>
   <si>
     <t>start</t>
+  </si>
+  <si>
+    <t>zone</t>
+  </si>
+  <si>
+    <t>specs</t>
+  </si>
+  <si>
+    <t>t</t>
+  </si>
+  <si>
+    <t>elevator</t>
+  </si>
+  <si>
+    <t>hall</t>
+  </si>
+  <si>
+    <t>closet</t>
+  </si>
+  <si>
+    <t>lockroom</t>
+  </si>
+  <si>
+    <t>skull</t>
+  </si>
+  <si>
+    <t>lights</t>
+  </si>
+  <si>
+    <t>music</t>
+  </si>
+  <si>
+    <t>security</t>
+  </si>
+  <si>
+    <t>arch</t>
+  </si>
+  <si>
+    <t>tesla</t>
+  </si>
+  <si>
+    <t>refine</t>
+  </si>
+  <si>
+    <t>sec hall</t>
+  </si>
+  <si>
+    <t>jumpers</t>
+  </si>
+  <si>
+    <t>rus mask</t>
+  </si>
+  <si>
+    <t>scps</t>
+  </si>
+  <si>
+    <t>basement</t>
+  </si>
+  <si>
+    <t>test</t>
+  </si>
+  <si>
+    <t>recurse</t>
+  </si>
+  <si>
+    <t>wallhole</t>
+  </si>
+  <si>
+    <t>rusmask</t>
+  </si>
+  <si>
+    <t>sechall</t>
+  </si>
+  <si>
+    <t>spcps</t>
+  </si>
+  <si>
+    <t xml:space="preserve">hall </t>
+  </si>
+  <si>
+    <t>Archives</t>
+  </si>
+  <si>
+    <t>Storeroom</t>
+  </si>
+  <si>
+    <t>Testing</t>
+  </si>
+  <si>
+    <t>Surveillance</t>
+  </si>
+  <si>
+    <t>SPCs</t>
   </si>
 </sst>
 </file>
@@ -102,9 +195,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -406,10 +500,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:O43"/>
+  <dimension ref="A1:Y45"/>
   <sheetViews>
-    <sheetView topLeftCell="A6" workbookViewId="0">
-      <selection sqref="A1:O43"/>
+    <sheetView tabSelected="1" topLeftCell="A21" workbookViewId="0">
+      <selection activeCell="R46" sqref="R46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -676,12 +770,12 @@
         <v>372</v>
       </c>
     </row>
-    <row r="17" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:25" x14ac:dyDescent="0.25">
       <c r="H17">
         <v>173</v>
       </c>
     </row>
-    <row r="25" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B25" t="s">
         <v>1</v>
       </c>
@@ -698,7 +792,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="26" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B26" t="s">
         <v>12</v>
       </c>
@@ -739,7 +833,7 @@
         <v>1162</v>
       </c>
     </row>
-    <row r="27" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="27" spans="2:25" x14ac:dyDescent="0.25">
       <c r="F27">
         <v>1499</v>
       </c>
@@ -750,7 +844,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="28" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="28" spans="2:25" x14ac:dyDescent="0.25">
       <c r="F28">
         <v>12</v>
       </c>
@@ -764,7 +858,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="29" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="29" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B29">
         <v>372</v>
       </c>
@@ -805,12 +899,49 @@
         <v>11</v>
       </c>
     </row>
-    <row r="30" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="30" spans="2:25" x14ac:dyDescent="0.25">
       <c r="H30">
         <v>173</v>
       </c>
     </row>
-    <row r="38" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="31" spans="2:25" x14ac:dyDescent="0.25">
+      <c r="T31">
+        <v>0</v>
+      </c>
+      <c r="U31">
+        <v>1</v>
+      </c>
+      <c r="V31">
+        <v>2</v>
+      </c>
+      <c r="W31">
+        <v>3</v>
+      </c>
+      <c r="X31">
+        <v>4</v>
+      </c>
+      <c r="Y31">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="36" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Q36">
+        <v>1</v>
+      </c>
+      <c r="S36">
+        <v>2</v>
+      </c>
+      <c r="U36">
+        <v>3</v>
+      </c>
+      <c r="W36" t="s">
+        <v>12</v>
+      </c>
+      <c r="Y36">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="38" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B38" t="s">
         <v>1</v>
       </c>
@@ -823,8 +954,20 @@
       <c r="I38" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="39" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="Q38">
+        <v>205</v>
+      </c>
+      <c r="S38">
+        <v>12</v>
+      </c>
+      <c r="U38">
+        <v>939</v>
+      </c>
+      <c r="W38">
+        <v>1162</v>
+      </c>
+    </row>
+    <row r="39" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>10</v>
       </c>
@@ -858,8 +1001,14 @@
       <c r="K39">
         <v>1162</v>
       </c>
-    </row>
-    <row r="40" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="Q39">
+        <v>372</v>
+      </c>
+      <c r="S39">
+        <v>970</v>
+      </c>
+    </row>
+    <row r="40" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B40" t="s">
         <v>2</v>
       </c>
@@ -869,8 +1018,14 @@
       <c r="K40">
         <v>1499</v>
       </c>
-    </row>
-    <row r="41" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="Q40">
+        <v>914</v>
+      </c>
+      <c r="S40">
+        <v>1123</v>
+      </c>
+    </row>
+    <row r="41" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B41">
         <v>12</v>
       </c>
@@ -886,8 +1041,14 @@
       <c r="M41">
         <v>914</v>
       </c>
-    </row>
-    <row r="42" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="Q41">
+        <v>178</v>
+      </c>
+      <c r="S41">
+        <v>1499</v>
+      </c>
+    </row>
+    <row r="42" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B42" t="s">
         <v>11</v>
       </c>
@@ -927,10 +1088,44 @@
       <c r="N42">
         <v>372</v>
       </c>
-    </row>
-    <row r="43" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="P42">
+        <v>10001</v>
+      </c>
+      <c r="Q42" t="s">
+        <v>41</v>
+      </c>
+      <c r="R42">
+        <v>20001</v>
+      </c>
+      <c r="S42" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="43" spans="1:25" x14ac:dyDescent="0.25">
       <c r="H43">
         <v>173</v>
+      </c>
+      <c r="R43">
+        <v>20002</v>
+      </c>
+      <c r="S43" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="44" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="R44">
+        <v>20003</v>
+      </c>
+      <c r="S44" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="45" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="R45">
+        <v>20004</v>
+      </c>
+      <c r="S45" t="s">
+        <v>45</v>
       </c>
     </row>
   </sheetData>
@@ -1502,10 +1697,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:O30"/>
+  <dimension ref="A1:O54"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="P23" sqref="P23"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="Y58" sqref="Y58"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2041,6 +2236,522 @@
         <v>173</v>
       </c>
     </row>
+    <row r="33" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="B33" s="2"/>
+      <c r="C33" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D33" s="2"/>
+      <c r="E33" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F33" s="2"/>
+      <c r="G33" s="2"/>
+      <c r="H33" s="2"/>
+      <c r="I33" s="2"/>
+      <c r="J33" s="2"/>
+      <c r="K33" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="L33" s="2"/>
+      <c r="M33" s="2"/>
+      <c r="N33" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="O33" s="2"/>
+    </row>
+    <row r="34" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="B34" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C34" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D34" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="E34" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="F34" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="G34" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="H34" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="I34" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="J34" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="K34" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="L34" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="M34" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="N34" s="1">
+        <v>4</v>
+      </c>
+      <c r="O34" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="35" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="B35" s="2"/>
+      <c r="C35" s="2"/>
+      <c r="D35" s="2"/>
+      <c r="E35" s="2"/>
+      <c r="F35" s="2"/>
+      <c r="G35" s="2"/>
+      <c r="H35" s="2"/>
+      <c r="I35" s="2"/>
+      <c r="J35" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="K35" s="2"/>
+      <c r="L35" s="2"/>
+      <c r="M35" s="2"/>
+      <c r="N35" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="O35" s="2"/>
+    </row>
+    <row r="36" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="B36" s="2"/>
+      <c r="C36" s="2"/>
+      <c r="D36" s="2"/>
+      <c r="E36" s="2"/>
+      <c r="F36" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="G36" s="2"/>
+      <c r="H36" s="2"/>
+      <c r="I36" s="2"/>
+      <c r="J36" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="K36" s="2"/>
+      <c r="L36" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="M36" s="2"/>
+      <c r="N36" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="O36" s="2"/>
+    </row>
+    <row r="37" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="B37" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C37" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D37" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="E37" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="F37" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="G37" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="H37" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="I37" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="J37" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="K37" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="L37" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="M37" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="N37" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="O37" s="2"/>
+    </row>
+    <row r="38" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="B38" s="2"/>
+      <c r="C38" s="2"/>
+      <c r="D38" s="2"/>
+      <c r="E38" s="2"/>
+      <c r="F38" s="2"/>
+      <c r="G38" s="2"/>
+      <c r="H38" s="1">
+        <v>173</v>
+      </c>
+      <c r="I38" s="2"/>
+      <c r="J38" s="2"/>
+      <c r="K38" s="2"/>
+      <c r="L38" s="2"/>
+      <c r="M38" s="2"/>
+      <c r="N38" s="2"/>
+      <c r="O38" s="2"/>
+    </row>
+    <row r="41" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A41" s="2"/>
+      <c r="B41" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C41" s="2"/>
+      <c r="D41" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="E41" s="2"/>
+      <c r="F41" s="2"/>
+      <c r="G41" s="2"/>
+      <c r="H41" s="2"/>
+      <c r="I41" s="2"/>
+      <c r="J41" s="2"/>
+      <c r="K41" s="2"/>
+      <c r="L41" s="2"/>
+      <c r="M41" s="2"/>
+      <c r="N41" s="2"/>
+      <c r="O41" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="42" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A42" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B42" s="1">
+        <v>4</v>
+      </c>
+      <c r="C42" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="D42" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="E42" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="F42" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="G42" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="H42" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="I42" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="J42" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="K42" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="L42" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="M42" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="N42" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="O42" s="1" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="43" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A43" s="2"/>
+      <c r="B43" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C43" s="2"/>
+      <c r="D43" s="2"/>
+      <c r="E43" s="2"/>
+      <c r="F43" s="2"/>
+      <c r="G43" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="H43" s="2"/>
+      <c r="I43" s="2"/>
+      <c r="J43" s="2"/>
+      <c r="K43" s="2"/>
+      <c r="L43" s="2"/>
+      <c r="M43" s="2"/>
+      <c r="N43" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="O43" s="2"/>
+    </row>
+    <row r="44" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A44" s="2"/>
+      <c r="B44" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="C44" s="2"/>
+      <c r="D44" s="2"/>
+      <c r="E44" s="2"/>
+      <c r="F44" s="2"/>
+      <c r="G44" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="H44" s="2"/>
+      <c r="I44" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="J44" s="2"/>
+      <c r="K44" s="2"/>
+      <c r="L44" s="2"/>
+      <c r="M44" s="2"/>
+      <c r="N44" s="2"/>
+      <c r="O44" s="2"/>
+    </row>
+    <row r="45" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A45" s="2"/>
+      <c r="B45" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C45" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="D45" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="E45" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="F45" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="G45" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="H45" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="I45" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="J45" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="K45" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="L45" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="M45" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="N45" s="2"/>
+      <c r="O45" s="2"/>
+    </row>
+    <row r="46" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A46" s="2"/>
+      <c r="B46" s="2"/>
+      <c r="C46" s="2"/>
+      <c r="D46" s="2"/>
+      <c r="E46" s="2"/>
+      <c r="F46" s="2"/>
+      <c r="G46" s="2"/>
+      <c r="H46" s="1">
+        <v>173</v>
+      </c>
+      <c r="I46" s="2"/>
+      <c r="J46" s="2"/>
+      <c r="K46" s="2"/>
+      <c r="L46" s="2"/>
+      <c r="M46" s="2"/>
+      <c r="N46" s="2"/>
+      <c r="O46" s="2"/>
+    </row>
+    <row r="49" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A49" s="2"/>
+      <c r="B49" s="2"/>
+      <c r="C49" s="2"/>
+      <c r="D49" s="2"/>
+      <c r="E49" s="2"/>
+      <c r="F49" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G49" s="2"/>
+      <c r="H49" s="2"/>
+      <c r="I49" s="2"/>
+      <c r="J49" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="K49" s="2"/>
+      <c r="L49" s="2"/>
+      <c r="M49" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="N49" s="2"/>
+      <c r="O49" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="50" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A50" s="2"/>
+      <c r="B50" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C50" s="1"/>
+      <c r="D50" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="E50" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="F50" s="1">
+        <v>4</v>
+      </c>
+      <c r="G50" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="H50" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="I50" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="J50" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="K50" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="L50" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="M50" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="N50" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="O50" s="1" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="51" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A51" s="2"/>
+      <c r="B51" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="C51" s="2"/>
+      <c r="D51" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="E51" s="2"/>
+      <c r="F51" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="G51" s="2"/>
+      <c r="H51" s="2"/>
+      <c r="I51" s="2"/>
+      <c r="J51" s="2"/>
+      <c r="K51" s="2"/>
+      <c r="L51" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="M51" s="2"/>
+      <c r="N51" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="O51" s="2"/>
+    </row>
+    <row r="52" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A52" s="2"/>
+      <c r="B52" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C52" s="2"/>
+      <c r="D52" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="E52" s="2"/>
+      <c r="F52" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="G52" s="2"/>
+      <c r="H52" s="2"/>
+      <c r="I52" s="2"/>
+      <c r="J52" s="2"/>
+      <c r="K52" s="2"/>
+      <c r="L52" s="2"/>
+      <c r="M52" s="2"/>
+      <c r="N52" s="2"/>
+      <c r="O52" s="2"/>
+    </row>
+    <row r="53" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A53" s="2"/>
+      <c r="B53" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C53" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="D53" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="E53" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="F53" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="G53" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="H53" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="I53" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="J53" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="K53" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="L53" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="M53" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="N53" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="O53" s="1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="54" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="H54" s="1">
+        <v>173</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>